<commit_message>
New files provided by Vincent
</commit_message>
<xml_diff>
--- a/patient_list.xlsx
+++ b/patient_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphaelbourque/Desktop/projet psychosis connectome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F1D4B2-25B5-E64A-B245-7DA0B92913A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3156566C-6CA1-E648-9C87-59DACEC38DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{D3B9D148-3985-B64D-9C83-F6D433740E32}"/>
+    <workbookView xWindow="520" yWindow="2480" windowWidth="28040" windowHeight="16420" xr2:uid="{D3B9D148-3985-B64D-9C83-F6D433740E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="184">
   <si>
     <t xml:space="preserve">Right cerebellar hemisphere </t>
   </si>
@@ -336,9 +336,6 @@
     <t>Precuneus Left</t>
   </si>
   <si>
-    <t>Angular Left</t>
-  </si>
-  <si>
     <t>SupraMarginal Left</t>
   </si>
   <si>
@@ -528,9 +525,6 @@
     <t>parietal</t>
   </si>
   <si>
-    <t>###</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cotard syndrome </t>
   </si>
   <si>
@@ -549,9 +543,6 @@
     <t>occipital</t>
   </si>
   <si>
-    <t>hippocampus</t>
-  </si>
-  <si>
     <t>fusiform</t>
   </si>
   <si>
@@ -582,13 +573,19 @@
     <t>olfactory</t>
   </si>
   <si>
-    <t>tempo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Persecutory delusions and visual hallucinations </t>
   </si>
   <si>
     <t xml:space="preserve">Psychosis unspecified </t>
+  </si>
+  <si>
+    <t>brainstem</t>
+  </si>
+  <si>
+    <t>hippocamp</t>
+  </si>
+  <si>
+    <t>Angular left</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B6F60F-DF36-F740-B692-911AB1271EA4}">
   <dimension ref="A1:BP62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B17" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="BR2" sqref="BR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1328,563 +1325,563 @@
         <v>99</v>
       </c>
       <c r="S1" t="s">
+        <v>183</v>
+      </c>
+      <c r="T1" t="s">
         <v>100</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>101</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>102</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>103</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>104</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>106</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>107</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>108</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>109</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>110</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>111</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>112</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>113</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>114</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>115</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>116</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>117</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>118</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>119</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>120</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>121</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>122</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>123</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>124</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>125</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>126</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>127</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>128</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>129</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>130</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>131</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>132</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>133</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>134</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>135</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>136</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>137</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>138</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>139</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>140</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>141</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>142</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>143</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>144</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>145</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>146</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>147</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>148</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
         <v>150</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>150</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>150</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" t="s">
         <v>151</v>
       </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>152</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>153</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>154</v>
       </c>
-      <c r="K2" t="s">
-        <v>164</v>
-      </c>
       <c r="L2" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="M2" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="N2" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="O2" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="P2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="S2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="T2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="U2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="V2" t="s">
+        <v>159</v>
+      </c>
+      <c r="W2" t="s">
+        <v>159</v>
+      </c>
+      <c r="X2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z2" t="s">
         <v>182</v>
       </c>
-      <c r="W2" t="s">
-        <v>160</v>
-      </c>
-      <c r="X2" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>164</v>
-      </c>
       <c r="AA2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AV2" t="s">
         <v>159</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AW2" t="s">
         <v>159</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AX2" t="s">
         <v>159</v>
       </c>
-      <c r="AD2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>157</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>157</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>167</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>168</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AQ2" t="s">
+      <c r="AY2" t="s">
         <v>170</v>
       </c>
-      <c r="AR2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AT2" t="s">
+      <c r="AZ2" t="s">
         <v>171</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BA2" t="s">
         <v>172</v>
       </c>
-      <c r="AV2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="BB2" t="s">
         <v>173</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BC2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BE2" t="s">
         <v>174</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BF2" t="s">
         <v>175</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BG2" t="s">
         <v>176</v>
       </c>
-      <c r="BC2" t="s">
-        <v>163</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>163</v>
-      </c>
-      <c r="BE2" t="s">
+      <c r="BH2" t="s">
         <v>177</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BI2" t="s">
+        <v>154</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>153</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BL2" t="s">
         <v>178</v>
       </c>
-      <c r="BG2" t="s">
-        <v>179</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>180</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>155</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>154</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>153</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>181</v>
-      </c>
       <c r="BM2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BN2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BO2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BP2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:68">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M3" t="s">
+        <v>160</v>
+      </c>
+      <c r="N3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O3" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>160</v>
+      </c>
+      <c r="R3" t="s">
+        <v>160</v>
+      </c>
+      <c r="S3" t="s">
+        <v>160</v>
+      </c>
+      <c r="T3" t="s">
+        <v>160</v>
+      </c>
+      <c r="U3" t="s">
+        <v>160</v>
+      </c>
+      <c r="V3" t="s">
+        <v>160</v>
+      </c>
+      <c r="W3" t="s">
+        <v>160</v>
+      </c>
+      <c r="X3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK3" t="s">
         <v>161</v>
       </c>
-      <c r="E3" t="s">
+      <c r="AL3" t="s">
         <v>161</v>
       </c>
-      <c r="F3" t="s">
+      <c r="AM3" t="s">
         <v>161</v>
       </c>
-      <c r="G3" t="s">
+      <c r="AN3" t="s">
         <v>161</v>
       </c>
-      <c r="H3" t="s">
+      <c r="AO3" t="s">
         <v>161</v>
       </c>
-      <c r="I3" t="s">
+      <c r="AP3" t="s">
         <v>161</v>
       </c>
-      <c r="J3" t="s">
+      <c r="AQ3" t="s">
         <v>161</v>
       </c>
-      <c r="K3" t="s">
+      <c r="AR3" t="s">
         <v>161</v>
       </c>
-      <c r="L3" t="s">
+      <c r="AS3" t="s">
         <v>161</v>
       </c>
-      <c r="M3" t="s">
+      <c r="AT3" t="s">
         <v>161</v>
       </c>
-      <c r="N3" t="s">
+      <c r="AU3" t="s">
         <v>161</v>
       </c>
-      <c r="O3" t="s">
+      <c r="AV3" t="s">
         <v>161</v>
       </c>
-      <c r="P3" t="s">
+      <c r="AW3" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="AX3" t="s">
         <v>161</v>
       </c>
-      <c r="R3" t="s">
+      <c r="AY3" t="s">
         <v>161</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AZ3" t="s">
         <v>161</v>
       </c>
-      <c r="T3" t="s">
+      <c r="BA3" t="s">
         <v>161</v>
       </c>
-      <c r="U3" t="s">
+      <c r="BB3" t="s">
         <v>161</v>
       </c>
-      <c r="V3" t="s">
+      <c r="BC3" t="s">
         <v>161</v>
       </c>
-      <c r="W3" t="s">
+      <c r="BD3" t="s">
         <v>161</v>
       </c>
-      <c r="X3" t="s">
+      <c r="BE3" t="s">
         <v>161</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="BF3" t="s">
         <v>161</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="BG3" t="s">
         <v>161</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="BH3" t="s">
         <v>161</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="BI3" t="s">
         <v>161</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="BJ3" t="s">
         <v>161</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="BK3" t="s">
         <v>161</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="BL3" t="s">
         <v>161</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="BM3" t="s">
         <v>161</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="BN3" t="s">
         <v>161</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="BO3" t="s">
         <v>161</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="BP3" t="s">
         <v>161</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -5415,7 +5412,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C17">
         <v>28</v>
@@ -6228,7 +6225,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C20">
         <v>72</v>
@@ -6578,7 +6575,7 @@
       </c>
       <c r="V21">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21">
         <f t="shared" si="4"/>
@@ -8938,7 +8935,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C30">
         <v>71</v>
@@ -10372,7 +10369,7 @@
       </c>
       <c r="V35">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W35">
         <f t="shared" si="7"/>
@@ -10643,7 +10640,7 @@
       </c>
       <c r="V36">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W36">
         <f t="shared" si="7"/>
@@ -10835,7 +10832,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C37">
         <v>55</v>
@@ -12014,7 +12011,7 @@
       </c>
       <c r="Z41">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA41">
         <f t="shared" si="7"/>
@@ -12732,7 +12729,7 @@
         <v>51</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C44">
         <v>73</v>
@@ -13353,7 +13350,7 @@
       </c>
       <c r="V46">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W46">
         <f t="shared" si="13"/>
@@ -15442,7 +15439,7 @@
         <v>64</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C54">
         <v>30</v>
@@ -15521,7 +15518,7 @@
       </c>
       <c r="V54">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W54">
         <f t="shared" si="13"/>

</xml_diff>